<commit_message>
added smaller file for testing
</commit_message>
<xml_diff>
--- a/excel_input_files/Test_input_Condition1Neg_Subset.xlsx
+++ b/excel_input_files/Test_input_Condition1Neg_Subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/git/lipid_prototype/excel_input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB603E7-FA8D-E644-84B7-C832144E7329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECE4DEA-8561-7040-B4BC-78AEC9E46049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30980" yWindow="1480" windowWidth="23260" windowHeight="12580" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
+    <workbookView xWindow="30980" yWindow="1480" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="lipids" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>abs</t>
+  </si>
+  <si>
+    <t>scan_delta</t>
   </si>
 </sst>
 </file>
@@ -562,8 +565,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1258,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C0786-739C-D54D-82F4-D057694BAA36}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,6 +1301,14 @@
         <v>34</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>